<commit_message>
US Finalization - Sprint B
</commit_message>
<xml_diff>
--- a/docs/Sprint-B/SprintB - Assessment.xlsx
+++ b/docs/Sprint-B/SprintB - Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\ISEP-1ºano-2º Semestre\lei-23-s2-1dj-g47\docs\Sprint-B\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9079e2d29d98ec5b/Ambiente de Trabalho/Rodrick/Ensino Superior/Trabalhos ISEP/APROG/Semana 4/lei-23-s2-1dj-g47/docs/Sprint-B/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19BAE69B-0026-460D-B7FC-2CB3CE85321E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{19BAE69B-0026-460D-B7FC-2CB3CE85321E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70989B2B-EAC5-4FF1-91A8-0EB9972609B9}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1229,6 +1229,10 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2671 24575,'0'-20'0,"0"1"0,0-12 0,0 4 0,0-9 0,0 7 0,0-17 0,0-27 0,0 26 0,0-33 0,0 42 0,0-1 0,0-8 0,6 18 0,2-17 0,6 17 0,0-7 0,-6 9 0,4 1 0,-11-1 0,9 8 0,-8-6 0,7 13 0,-8-5 0,3 6 0,-4-6 0,26-37 0,-14 19 0,20-30 0,-21 44 0,1-8 0,-6 17 0,6-13 0,-11 13 0,11-13 0,-6 13 0,7-12 0,-1 4 0,1-6 0,0-1 0,0 1 0,1-1 0,0-9 0,-1 14 0,1-13 0,-2 16 0,0 0 0,-1 1 0,1 1 0,-2 5 0,14-7 0,-5-3 0,4 7 0,1-8 0,-12 12 0,13-2 0,-13 3 0,12-9 0,-12 7 0,13-7 0,-6 1 0,55-19 0,9-2 0,-24 5 0,22-3 0,-6 5 0,-48 20 0,11 5 0,-9-6 0,9 0 0,-11 5 0,-8-2 0,6 9 0,-6-4 0,18-2 0,-8-1 0,7-6 0,-10 0 0,1 7 0,-8-3 0,6 8 0,-1-7 0,3 8 0,-3-8 0,1 8 0,-13-4 0,13 5 0,-13 0 0,12-6 0,-11 5 0,16-5 0,-9 0 0,4 5 0,1-5 0,-6 0 0,0 4 0,6-9 0,-6 9 0,1-4 0,-3 6 0,-7-4 0,8 3 0,-6-4 0,5 5 0,-6 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,8 0 0,-6 0 0,5 0 0,-7 0 0,1 0 0,-2 0 0,-7 0 0,-11-6 0,-9-1 0,-1-5 0,-16-2 0,10-3 0,-6 3 0,3-9 0,8 9 0,1-3 0,0-2 0,9 7 0,-3-13 0,1 6 0,-10-18 0,7 8 0,-13-7 0,12 0 0,-3 7 0,-2-7 0,6 9 0,-19-2 0,10 8 0,-5 5 0,5 4 0,12 6 0,-6-6 0,1 7 0,4-5 0,-4 9 0,7-8 0,-1 3 0,1-4 0,0 5 0,0-5 0,-10 0 0,9 3 0,-4-6 0,7 11 0,7-6 0,1 11 0,5-1 0,4 7 0,1 1 0,2 8 0,16 4 0,-5-1 0,13 1 0,-9-3 0,9-3 0,-7 3 0,7-4 0,-15 4 0,4-4 0,-12 2 0,5-5 0,-8-2 0,0 1 0,1-1 0,0 7 0,0-5 0,0 6 0,1-1 0,-1-5 0,0 6 0,-1-8 0,-4 8 0,3-6 0,3 17 0,-5-16 0,3 16 0,-10-17 0,6 13 0,-4-13 0,14 17 0,-14-16 0,9 9 0,-5-4 0,-5-6 0,10 5 0,-10-6 0,3-1 0,1 0 0,-4 0 0,4 1 0,-2-6 0,1 0 0,4-5 0,0 0 0,1 0 0,0 0 0,8 0 0,-5 0 0,12 0 0,-12 0 0,6 0 0,-8 0 0,0 0 0,0 0 0,-4 3 0,-6-2 0,-6 7 0,-10-7 0,4 8 0,-13-2 0,6 5 0,-2 7 0,-4-4 0,4 4 0,1 0 0,-5-4 0,11 3 0,-10 0 0,10 2 0,-3-1 0,4 5 0,0 6 0,-21 20 0,13 2 0,-22 8 0,25-11 0,-12 0 0,13-10 0,-5-3 0,9-9 0,5-8 0,-2-1 0,9-8 0,-4 0 0,5 0 0,-3-4 0,-2 3 0,-4-3 0,-2 4 0,1 0 0,0 1 0,4-1 0,-3 0 0,8 0 0,-4 0 0,1-4 0,3-2 0,-4-4 0</inkml:trace>
 </inkml:ink>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1532,10 +1536,10 @@
   <dimension ref="A1:T39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -1543,19 +1547,19 @@
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="33.5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.7">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1566,7 +1570,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="76"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1574,7 +1578,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1582,7 +1586,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1590,7 +1594,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1600,7 +1604,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1610,7 +1614,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1620,7 +1624,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1630,7 +1634,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1640,7 +1644,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1650,29 +1654,31 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="9"/>
+      <c r="B14" s="9">
+        <v>47</v>
+      </c>
       <c r="C14" s="7" t="s">
         <v>13</v>
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1680,8 +1686,8 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="18" spans="2:20" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="18" spans="2:20" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="77" t="s">
@@ -1703,7 +1709,7 @@
       <c r="S18" s="78"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="2:20" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="13">
@@ -1770,7 +1776,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B20" s="80" t="s">
         <v>17</v>
       </c>
@@ -1807,16 +1813,26 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B21" s="81"/>
       <c r="C21" s="21">
         <v>1220741</v>
       </c>
-      <c r="D21" s="22"/>
-      <c r="E21" s="17"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
+      <c r="D21" s="22">
+        <v>3</v>
+      </c>
+      <c r="E21" s="17">
+        <v>4</v>
+      </c>
+      <c r="F21" s="23">
+        <v>4</v>
+      </c>
+      <c r="G21" s="21">
+        <v>4</v>
+      </c>
+      <c r="H21" s="21">
+        <v>4</v>
+      </c>
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
       <c r="K21" s="21"/>
@@ -1827,21 +1843,31 @@
       <c r="P21" s="21"/>
       <c r="Q21" s="21"/>
       <c r="R21" s="24"/>
-      <c r="S21" s="25" t="e">
+      <c r="S21" s="25">
         <f t="shared" ref="S21:S34" si="0">AVERAGE(D21:R21)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B22" s="81"/>
       <c r="C22" s="21">
         <v>1221083</v>
       </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
-      <c r="F22" s="17"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="21"/>
+      <c r="D22" s="21">
+        <v>5</v>
+      </c>
+      <c r="E22" s="22">
+        <v>3</v>
+      </c>
+      <c r="F22" s="17">
+        <v>5</v>
+      </c>
+      <c r="G22" s="23">
+        <v>4</v>
+      </c>
+      <c r="H22" s="21">
+        <v>4</v>
+      </c>
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
       <c r="K22" s="21"/>
@@ -1852,12 +1878,12 @@
       <c r="P22" s="21"/>
       <c r="Q22" s="21"/>
       <c r="R22" s="24"/>
-      <c r="S22" s="25" t="e">
+      <c r="S22" s="25">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="23" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="23" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="81"/>
       <c r="C23" s="21">
         <v>1220928</v>
@@ -1882,7 +1908,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>1220917</v>
@@ -1917,7 +1943,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B25" s="81"/>
       <c r="C25" s="21" t="s">
         <v>18</v>
@@ -1942,7 +1968,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B26" s="81"/>
       <c r="C26" s="21" t="s">
         <v>19</v>
@@ -1967,7 +1993,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" s="81"/>
       <c r="C27" s="21" t="s">
         <v>20</v>
@@ -1992,7 +2018,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B28" s="81"/>
       <c r="C28" s="21" t="s">
         <v>21</v>
@@ -2017,7 +2043,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B29" s="81"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -2042,7 +2068,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B30" s="81"/>
       <c r="C30" s="21" t="s">
         <v>23</v>
@@ -2067,7 +2093,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B31" s="81"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
@@ -2092,7 +2118,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B32" s="81"/>
       <c r="C32" s="21" t="s">
         <v>25</v>
@@ -2117,7 +2143,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B33" s="81"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2142,7 +2168,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B34" s="82"/>
       <c r="C34" s="27" t="s">
         <v>27</v>
@@ -2167,7 +2193,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
         <v>16</v>
@@ -2178,11 +2204,11 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" ref="E35:R35" si="1">AVERAGE(E20:E34)</f>
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="G35" s="31">
         <f t="shared" si="1"/>
@@ -2234,10 +2260,10 @@
       </c>
       <c r="S35" s="33"/>
     </row>
-    <row r="37" spans="1:19" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.7">
       <c r="A37" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A39" s="34"/>
     </row>
   </sheetData>
@@ -2263,10 +2289,10 @@
   <dimension ref="A1:AC18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="N11" sqref="N11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="11" style="73"/>
     <col min="4" max="23" width="7.25" style="74" customWidth="1"/>
@@ -2278,7 +2304,7 @@
     <col min="30" max="16384" width="11" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="40" customFormat="1" ht="343.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" s="40" customFormat="1" ht="343.9" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="35"/>
@@ -2359,7 +2385,7 @@
       </c>
       <c r="AC1" s="39"/>
     </row>
-    <row r="2" spans="1:29" s="40" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" s="40" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -2448,55 +2474,87 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="83" t="s">
         <v>60</v>
       </c>
       <c r="B3" s="83">
         <f>'Group and Self Assessment'!B14</f>
-        <v>0</v>
-      </c>
-      <c r="C3" s="46"/>
-      <c r="D3" s="47"/>
+        <v>47</v>
+      </c>
+      <c r="C3" s="46">
+        <v>1221083</v>
+      </c>
+      <c r="D3" s="47">
+        <v>4</v>
+      </c>
       <c r="E3" s="48"/>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
+      <c r="F3" s="47">
+        <v>4</v>
+      </c>
+      <c r="G3" s="47">
+        <v>4</v>
+      </c>
       <c r="H3" s="48"/>
       <c r="I3" s="48"/>
       <c r="J3" s="48"/>
-      <c r="K3" s="47"/>
-      <c r="L3" s="47"/>
-      <c r="M3" s="47"/>
-      <c r="N3" s="47"/>
-      <c r="O3" s="47"/>
-      <c r="P3" s="47"/>
-      <c r="Q3" s="47"/>
+      <c r="K3" s="47">
+        <v>4</v>
+      </c>
+      <c r="L3" s="47">
+        <v>4</v>
+      </c>
+      <c r="M3" s="47">
+        <v>4</v>
+      </c>
+      <c r="N3" s="47">
+        <v>4</v>
+      </c>
+      <c r="O3" s="47">
+        <v>4</v>
+      </c>
+      <c r="P3" s="47">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="47">
+        <v>4</v>
+      </c>
       <c r="R3" s="48"/>
       <c r="S3" s="48"/>
-      <c r="T3" s="47"/>
-      <c r="U3" s="47"/>
-      <c r="V3" s="47"/>
-      <c r="W3" s="47"/>
+      <c r="T3" s="47">
+        <v>4</v>
+      </c>
+      <c r="U3" s="47">
+        <v>4</v>
+      </c>
+      <c r="V3" s="47">
+        <v>4</v>
+      </c>
+      <c r="W3" s="47">
+        <v>4</v>
+      </c>
       <c r="X3" s="49"/>
       <c r="Y3" s="50">
         <f>SUMPRODUCT(D2:W2,D3:W3)/5</f>
-        <v>0</v>
+        <v>0.80000000000000016</v>
       </c>
       <c r="Z3" s="51">
         <f>Y3*5</f>
-        <v>0</v>
+        <v>4.0000000000000009</v>
       </c>
       <c r="AA3" s="52">
         <f>MIN(ROUND(Y3*20,2),20)</f>
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="AB3" s="53"/>
       <c r="AC3" s="54"/>
     </row>
-    <row r="4" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
-      <c r="C4" s="55"/>
+      <c r="C4" s="55">
+        <v>1220917</v>
+      </c>
       <c r="D4" s="56"/>
       <c r="E4" s="57"/>
       <c r="F4" s="56"/>
@@ -2533,50 +2591,82 @@
       <c r="AB4" s="62"/>
       <c r="AC4" s="63"/>
     </row>
-    <row r="5" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
-      <c r="C5" s="55"/>
-      <c r="D5" s="56"/>
+      <c r="C5" s="55">
+        <v>1220741</v>
+      </c>
+      <c r="D5" s="56">
+        <v>4</v>
+      </c>
       <c r="E5" s="57"/>
-      <c r="F5" s="56"/>
-      <c r="G5" s="56"/>
+      <c r="F5" s="56">
+        <v>3</v>
+      </c>
+      <c r="G5" s="56">
+        <v>5</v>
+      </c>
       <c r="H5" s="57"/>
       <c r="I5" s="57"/>
       <c r="J5" s="57"/>
-      <c r="K5" s="56"/>
-      <c r="L5" s="56"/>
-      <c r="M5" s="56"/>
-      <c r="N5" s="56"/>
-      <c r="O5" s="56"/>
-      <c r="P5" s="56"/>
-      <c r="Q5" s="56"/>
+      <c r="K5" s="56">
+        <v>3</v>
+      </c>
+      <c r="L5" s="56">
+        <v>4</v>
+      </c>
+      <c r="M5" s="56">
+        <v>4</v>
+      </c>
+      <c r="N5" s="56">
+        <v>3</v>
+      </c>
+      <c r="O5" s="56">
+        <v>4</v>
+      </c>
+      <c r="P5" s="56">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="56">
+        <v>3</v>
+      </c>
       <c r="R5" s="57"/>
       <c r="S5" s="57"/>
-      <c r="T5" s="56"/>
-      <c r="U5" s="56"/>
-      <c r="V5" s="56"/>
-      <c r="W5" s="56"/>
+      <c r="T5" s="56">
+        <v>3</v>
+      </c>
+      <c r="U5" s="56">
+        <v>4</v>
+      </c>
+      <c r="V5" s="56">
+        <v>4</v>
+      </c>
+      <c r="W5" s="56">
+        <v>2</v>
+      </c>
       <c r="X5" s="58"/>
       <c r="Y5" s="59">
         <f>SUMPRODUCT(D2:W2,D5:W5)/5</f>
-        <v>0</v>
+        <v>0.66000000000000014</v>
       </c>
       <c r="Z5" s="60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3000000000000007</v>
       </c>
       <c r="AA5" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.2</v>
       </c>
       <c r="AB5" s="62"/>
       <c r="AC5" s="63"/>
     </row>
-    <row r="6" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="84"/>
       <c r="B6" s="84"/>
-      <c r="C6" s="55"/>
+      <c r="C6" s="55">
+        <v>1211121</v>
+      </c>
       <c r="D6" s="56"/>
       <c r="E6" s="57"/>
       <c r="F6" s="56"/>
@@ -2613,10 +2703,12 @@
       <c r="AB6" s="62"/>
       <c r="AC6" s="63"/>
     </row>
-    <row r="7" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
-      <c r="C7" s="55"/>
+      <c r="C7" s="55">
+        <v>1220928</v>
+      </c>
       <c r="D7" s="56"/>
       <c r="E7" s="57"/>
       <c r="F7" s="56"/>
@@ -2653,7 +2745,7 @@
       <c r="AB7" s="62"/>
       <c r="AC7" s="63"/>
     </row>
-    <row r="8" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
       <c r="C8" s="64"/>
@@ -2693,7 +2785,7 @@
       <c r="AB8" s="71"/>
       <c r="AC8" s="72"/>
     </row>
-    <row r="10" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.7">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2704,7 +2796,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -2715,7 +2807,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A12" s="6" t="s">
         <v>62</v>
       </c>
@@ -2726,7 +2818,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -2739,7 +2831,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -2752,7 +2844,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2765,7 +2857,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -2778,7 +2870,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -2791,7 +2883,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2821,26 +2913,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8B18F131359BB48BCDE011E677140C8" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c575d82af674a11f8850f3227e50b0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40f68083-8b1e-401a-aff0-261d16eabb01" xmlns:ns3="6fb2d6cf-5937-415c-8e29-0a2ba0894026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee7e4bd6e2ea6e83e9fae13acd7478ae" ns2:_="" ns3:_="">
     <xsd:import namespace="40f68083-8b1e-401a-aff0-261d16eabb01"/>
@@ -3029,10 +3101,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DAA54B-90F9-4C2D-87EC-856BE0A86E6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
+    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3055,20 +3158,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DAA54B-90F9-4C2D-87EC-856BE0A86E6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
-    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
US001- assessement: Sprint B
</commit_message>
<xml_diff>
--- a/docs/Sprint-B/SprintB - Assessment.xlsx
+++ b/docs/Sprint-B/SprintB - Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9079e2d29d98ec5b/Ambiente de Trabalho/Rodrick/Ensino Superior/Trabalhos ISEP/APROG/Semana 4/lei-23-s2-1dj-g47/docs/Sprint-B/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\renat\IdeaProjects\lei-23-s2-1dj-g47\docs\Sprint-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{19BAE69B-0026-460D-B7FC-2CB3CE85321E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70989B2B-EAC5-4FF1-91A8-0EB9972609B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E845B741-AEDF-46F0-BF5A-6F46377E9FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17496" activeTab="1" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1229,10 +1229,6 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2671 24575,'0'-20'0,"0"1"0,0-12 0,0 4 0,0-9 0,0 7 0,0-17 0,0-27 0,0 26 0,0-33 0,0 42 0,0-1 0,0-8 0,6 18 0,2-17 0,6 17 0,0-7 0,-6 9 0,4 1 0,-11-1 0,9 8 0,-8-6 0,7 13 0,-8-5 0,3 6 0,-4-6 0,26-37 0,-14 19 0,20-30 0,-21 44 0,1-8 0,-6 17 0,6-13 0,-11 13 0,11-13 0,-6 13 0,7-12 0,-1 4 0,1-6 0,0-1 0,0 1 0,1-1 0,0-9 0,-1 14 0,1-13 0,-2 16 0,0 0 0,-1 1 0,1 1 0,-2 5 0,14-7 0,-5-3 0,4 7 0,1-8 0,-12 12 0,13-2 0,-13 3 0,12-9 0,-12 7 0,13-7 0,-6 1 0,55-19 0,9-2 0,-24 5 0,22-3 0,-6 5 0,-48 20 0,11 5 0,-9-6 0,9 0 0,-11 5 0,-8-2 0,6 9 0,-6-4 0,18-2 0,-8-1 0,7-6 0,-10 0 0,1 7 0,-8-3 0,6 8 0,-1-7 0,3 8 0,-3-8 0,1 8 0,-13-4 0,13 5 0,-13 0 0,12-6 0,-11 5 0,16-5 0,-9 0 0,4 5 0,1-5 0,-6 0 0,0 4 0,6-9 0,-6 9 0,1-4 0,-3 6 0,-7-4 0,8 3 0,-6-4 0,5 5 0,-6 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,8 0 0,-6 0 0,5 0 0,-7 0 0,1 0 0,-2 0 0,-7 0 0,-11-6 0,-9-1 0,-1-5 0,-16-2 0,10-3 0,-6 3 0,3-9 0,8 9 0,1-3 0,0-2 0,9 7 0,-3-13 0,1 6 0,-10-18 0,7 8 0,-13-7 0,12 0 0,-3 7 0,-2-7 0,6 9 0,-19-2 0,10 8 0,-5 5 0,5 4 0,12 6 0,-6-6 0,1 7 0,4-5 0,-4 9 0,7-8 0,-1 3 0,1-4 0,0 5 0,0-5 0,-10 0 0,9 3 0,-4-6 0,7 11 0,7-6 0,1 11 0,5-1 0,4 7 0,1 1 0,2 8 0,16 4 0,-5-1 0,13 1 0,-9-3 0,9-3 0,-7 3 0,7-4 0,-15 4 0,4-4 0,-12 2 0,5-5 0,-8-2 0,0 1 0,1-1 0,0 7 0,0-5 0,0 6 0,1-1 0,-1-5 0,0 6 0,-1-8 0,-4 8 0,3-6 0,3 17 0,-5-16 0,3 16 0,-10-17 0,6 13 0,-4-13 0,14 17 0,-14-16 0,9 9 0,-5-4 0,-5-6 0,10 5 0,-10-6 0,3-1 0,1 0 0,-4 0 0,4 1 0,-2-6 0,1 0 0,4-5 0,0 0 0,1 0 0,0 0 0,8 0 0,-5 0 0,12 0 0,-12 0 0,6 0 0,-8 0 0,0 0 0,0 0 0,-4 3 0,-6-2 0,-6 7 0,-10-7 0,4 8 0,-13-2 0,6 5 0,-2 7 0,-4-4 0,4 4 0,1 0 0,-5-4 0,11 3 0,-10 0 0,10 2 0,-3-1 0,4 5 0,0 6 0,-21 20 0,13 2 0,-22 8 0,25-11 0,-12 0 0,13-10 0,-5-3 0,9-9 0,5-8 0,-2-1 0,9-8 0,-4 0 0,5 0 0,-3-4 0,-2 3 0,-4-3 0,-2 4 0,1 0 0,0 1 0,4-1 0,-3 0 0,8 0 0,-4 0 0,1-4 0,3-2 0,-4-4 0</inkml:trace>
 </inkml:ink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1535,31 +1531,31 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.69921875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="19" width="7.75" customWidth="1"/>
+    <col min="4" max="19" width="7.69921875" customWidth="1"/>
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="33.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1570,7 +1566,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="76"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1578,7 +1574,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1586,7 +1582,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1594,7 +1590,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1604,7 +1600,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1614,7 +1610,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1624,7 +1620,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1634,7 +1630,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1644,7 +1640,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1654,13 +1650,13 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1672,13 +1668,13 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1686,8 +1682,8 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="2:20" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="18" spans="2:20" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="77" t="s">
@@ -1709,7 +1705,7 @@
       <c r="S18" s="78"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="2:20" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:20" ht="106.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="13">
@@ -1776,7 +1772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="80" t="s">
         <v>17</v>
       </c>
@@ -1813,7 +1809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="81"/>
       <c r="C21" s="21">
         <v>1220741</v>
@@ -1848,7 +1844,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="81"/>
       <c r="C22" s="21">
         <v>1221083</v>
@@ -1883,16 +1879,26 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="81"/>
       <c r="C23" s="21">
         <v>1220928</v>
       </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="21"/>
-      <c r="F23" s="22"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="23"/>
+      <c r="D23" s="21">
+        <v>4</v>
+      </c>
+      <c r="E23" s="21">
+        <v>4</v>
+      </c>
+      <c r="F23" s="22">
+        <v>4</v>
+      </c>
+      <c r="G23" s="17">
+        <v>4</v>
+      </c>
+      <c r="H23" s="23">
+        <v>4</v>
+      </c>
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
       <c r="K23" s="21"/>
@@ -1903,12 +1909,12 @@
       <c r="P23" s="21"/>
       <c r="Q23" s="21"/>
       <c r="R23" s="24"/>
-      <c r="S23" s="25" t="e">
+      <c r="S23" s="25">
         <f t="shared" si="0"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="24" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>1220917</v>
@@ -1943,7 +1949,7 @@
         <v>3.6</v>
       </c>
     </row>
-    <row r="25" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="25" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="81"/>
       <c r="C25" s="21" t="s">
         <v>18</v>
@@ -1968,7 +1974,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="81"/>
       <c r="C26" s="21" t="s">
         <v>19</v>
@@ -1993,7 +1999,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="81"/>
       <c r="C27" s="21" t="s">
         <v>20</v>
@@ -2018,7 +2024,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B28" s="81"/>
       <c r="C28" s="21" t="s">
         <v>21</v>
@@ -2043,7 +2049,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="81"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -2068,7 +2074,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B30" s="81"/>
       <c r="C30" s="21" t="s">
         <v>23</v>
@@ -2093,7 +2099,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="81"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
@@ -2118,7 +2124,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="81"/>
       <c r="C32" s="21" t="s">
         <v>25</v>
@@ -2143,7 +2149,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="81"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2168,7 +2174,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="82"/>
       <c r="C34" s="27" t="s">
         <v>27</v>
@@ -2193,7 +2199,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:19" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
         <v>16</v>
@@ -2204,11 +2210,11 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" ref="E35:R35" si="1">AVERAGE(E20:E34)</f>
-        <v>3.25</v>
+        <v>3.4</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="1"/>
-        <v>4.25</v>
+        <v>4.2</v>
       </c>
       <c r="G35" s="31">
         <f t="shared" si="1"/>
@@ -2260,10 +2266,10 @@
       </c>
       <c r="S35" s="33"/>
     </row>
-    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.7">
+    <row r="37" spans="1:19" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A37" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A39" s="34"/>
     </row>
   </sheetData>
@@ -2288,23 +2294,23 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="11" style="73"/>
-    <col min="4" max="23" width="7.25" style="74" customWidth="1"/>
+    <col min="4" max="23" width="7.19921875" style="74" customWidth="1"/>
     <col min="24" max="24" width="11" style="74"/>
     <col min="25" max="26" width="11" style="73"/>
     <col min="27" max="27" width="11" style="75"/>
-    <col min="28" max="28" width="13.25" style="74" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.19921875" style="74" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="35" style="74" customWidth="1"/>
     <col min="30" max="16384" width="11" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="40" customFormat="1" ht="343.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="40" customFormat="1" ht="343.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="35"/>
@@ -2385,7 +2391,7 @@
       </c>
       <c r="AC1" s="39"/>
     </row>
-    <row r="2" spans="1:29" s="40" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" s="40" customFormat="1" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -2474,7 +2480,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="83" t="s">
         <v>60</v>
       </c>
@@ -2549,7 +2555,7 @@
       <c r="AB3" s="53"/>
       <c r="AC3" s="54"/>
     </row>
-    <row r="4" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
       <c r="C4" s="55">
@@ -2591,7 +2597,7 @@
       <c r="AB4" s="62"/>
       <c r="AC4" s="63"/>
     </row>
-    <row r="5" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
       <c r="C5" s="55">
@@ -2661,7 +2667,7 @@
       <c r="AB5" s="62"/>
       <c r="AC5" s="63"/>
     </row>
-    <row r="6" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="84"/>
       <c r="B6" s="84"/>
       <c r="C6" s="55">
@@ -2703,49 +2709,77 @@
       <c r="AB6" s="62"/>
       <c r="AC6" s="63"/>
     </row>
-    <row r="7" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" customFormat="1" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
       <c r="C7" s="55">
         <v>1220928</v>
       </c>
-      <c r="D7" s="56"/>
+      <c r="D7" s="56">
+        <v>4</v>
+      </c>
       <c r="E7" s="57"/>
-      <c r="F7" s="56"/>
-      <c r="G7" s="56"/>
+      <c r="F7" s="56">
+        <v>3</v>
+      </c>
+      <c r="G7" s="56">
+        <v>4</v>
+      </c>
       <c r="H7" s="57"/>
       <c r="I7" s="57"/>
       <c r="J7" s="57"/>
-      <c r="K7" s="56"/>
-      <c r="L7" s="56"/>
-      <c r="M7" s="56"/>
-      <c r="N7" s="56"/>
-      <c r="O7" s="56"/>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
+      <c r="K7" s="56">
+        <v>3</v>
+      </c>
+      <c r="L7" s="56">
+        <v>3</v>
+      </c>
+      <c r="M7" s="56">
+        <v>3</v>
+      </c>
+      <c r="N7" s="56">
+        <v>4</v>
+      </c>
+      <c r="O7" s="56">
+        <v>3</v>
+      </c>
+      <c r="P7" s="56">
+        <v>3</v>
+      </c>
+      <c r="Q7" s="56">
+        <v>3</v>
+      </c>
       <c r="R7" s="57"/>
       <c r="S7" s="57"/>
-      <c r="T7" s="56"/>
-      <c r="U7" s="56"/>
-      <c r="V7" s="56"/>
-      <c r="W7" s="56"/>
+      <c r="T7" s="56">
+        <v>4</v>
+      </c>
+      <c r="U7" s="56">
+        <v>3</v>
+      </c>
+      <c r="V7" s="56">
+        <v>3</v>
+      </c>
+      <c r="W7" s="56">
+        <v>3</v>
+      </c>
       <c r="X7" s="58"/>
       <c r="Y7" s="59">
         <f>SUMPRODUCT(D2:W2,D7:W7)/5</f>
-        <v>0</v>
+        <v>0.67090909090909101</v>
       </c>
       <c r="Z7" s="60">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3.3545454545454549</v>
       </c>
       <c r="AA7" s="61">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>13.42</v>
       </c>
       <c r="AB7" s="62"/>
       <c r="AC7" s="63"/>
     </row>
-    <row r="8" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:29" customFormat="1" ht="19.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
       <c r="C8" s="64"/>
@@ -2785,7 +2819,7 @@
       <c r="AB8" s="71"/>
       <c r="AC8" s="72"/>
     </row>
-    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:29" ht="31.2" x14ac:dyDescent="0.6">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2796,7 +2830,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -2807,7 +2841,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>62</v>
       </c>
@@ -2818,7 +2852,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -2831,7 +2865,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -2844,7 +2878,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2857,7 +2891,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" ht="18" x14ac:dyDescent="0.3">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -2870,7 +2904,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -2883,7 +2917,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.3">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2913,6 +2947,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8B18F131359BB48BCDE011E677140C8" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c575d82af674a11f8850f3227e50b0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40f68083-8b1e-401a-aff0-261d16eabb01" xmlns:ns3="6fb2d6cf-5937-415c-8e29-0a2ba0894026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee7e4bd6e2ea6e83e9fae13acd7478ae" ns2:_="" ns3:_="">
     <xsd:import namespace="40f68083-8b1e-401a-aff0-261d16eabb01"/>
@@ -3101,41 +3155,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DAA54B-90F9-4C2D-87EC-856BE0A86E6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
-    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3158,9 +3181,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DAA54B-90F9-4C2D-87EC-856BE0A86E6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
+    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
assessment sprint B correction of an error on sd readme conclusion
</commit_message>
<xml_diff>
--- a/docs/Sprint-B/SprintB - Assessment.xlsx
+++ b/docs/Sprint-B/SprintB - Assessment.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9079e2d29d98ec5b/Ambiente de Trabalho/Rodrick/Ensino Superior/Trabalhos ISEP/APROG/Semana 4/lei-23-s2-1dj-g47/docs/Sprint-B/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomas\OneDrive\Ambiente de Trabalho\ISEP-1ºano-2º Semestre\lei-23-s2-1dj-g47\docs\Sprint-B\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="55" documentId="13_ncr:1_{19BAE69B-0026-460D-B7FC-2CB3CE85321E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70989B2B-EAC5-4FF1-91A8-0EB9972609B9}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892A1370-9495-4F7C-A691-CEF0DD743B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" activeTab="1" xr2:uid="{C9F9D952-C72F-9A4E-AE70-234088236500}"/>
   </bookViews>
   <sheets>
     <sheet name="Group and Self Assessment" sheetId="2" r:id="rId1"/>
@@ -1229,10 +1229,6 @@
   </inkml:definitions>
   <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2671 24575,'0'-20'0,"0"1"0,0-12 0,0 4 0,0-9 0,0 7 0,0-17 0,0-27 0,0 26 0,0-33 0,0 42 0,0-1 0,0-8 0,6 18 0,2-17 0,6 17 0,0-7 0,-6 9 0,4 1 0,-11-1 0,9 8 0,-8-6 0,7 13 0,-8-5 0,3 6 0,-4-6 0,26-37 0,-14 19 0,20-30 0,-21 44 0,1-8 0,-6 17 0,6-13 0,-11 13 0,11-13 0,-6 13 0,7-12 0,-1 4 0,1-6 0,0-1 0,0 1 0,1-1 0,0-9 0,-1 14 0,1-13 0,-2 16 0,0 0 0,-1 1 0,1 1 0,-2 5 0,14-7 0,-5-3 0,4 7 0,1-8 0,-12 12 0,13-2 0,-13 3 0,12-9 0,-12 7 0,13-7 0,-6 1 0,55-19 0,9-2 0,-24 5 0,22-3 0,-6 5 0,-48 20 0,11 5 0,-9-6 0,9 0 0,-11 5 0,-8-2 0,6 9 0,-6-4 0,18-2 0,-8-1 0,7-6 0,-10 0 0,1 7 0,-8-3 0,6 8 0,-1-7 0,3 8 0,-3-8 0,1 8 0,-13-4 0,13 5 0,-13 0 0,12-6 0,-11 5 0,16-5 0,-9 0 0,4 5 0,1-5 0,-6 0 0,0 4 0,6-9 0,-6 9 0,1-4 0,-3 6 0,-7-4 0,8 3 0,-6-4 0,5 5 0,-6 0 0,-1 0 0,0 0 0,0 0 0,1 0 0,-1 0 0,0 0 0,8 0 0,-6 0 0,5 0 0,-7 0 0,1 0 0,-2 0 0,-7 0 0,-11-6 0,-9-1 0,-1-5 0,-16-2 0,10-3 0,-6 3 0,3-9 0,8 9 0,1-3 0,0-2 0,9 7 0,-3-13 0,1 6 0,-10-18 0,7 8 0,-13-7 0,12 0 0,-3 7 0,-2-7 0,6 9 0,-19-2 0,10 8 0,-5 5 0,5 4 0,12 6 0,-6-6 0,1 7 0,4-5 0,-4 9 0,7-8 0,-1 3 0,1-4 0,0 5 0,0-5 0,-10 0 0,9 3 0,-4-6 0,7 11 0,7-6 0,1 11 0,5-1 0,4 7 0,1 1 0,2 8 0,16 4 0,-5-1 0,13 1 0,-9-3 0,9-3 0,-7 3 0,7-4 0,-15 4 0,4-4 0,-12 2 0,5-5 0,-8-2 0,0 1 0,1-1 0,0 7 0,0-5 0,0 6 0,1-1 0,-1-5 0,0 6 0,-1-8 0,-4 8 0,3-6 0,3 17 0,-5-16 0,3 16 0,-10-17 0,6 13 0,-4-13 0,14 17 0,-14-16 0,9 9 0,-5-4 0,-5-6 0,10 5 0,-10-6 0,3-1 0,1 0 0,-4 0 0,4 1 0,-2-6 0,1 0 0,4-5 0,0 0 0,1 0 0,0 0 0,8 0 0,-5 0 0,12 0 0,-12 0 0,6 0 0,-8 0 0,0 0 0,0 0 0,-4 3 0,-6-2 0,-6 7 0,-10-7 0,4 8 0,-13-2 0,6 5 0,-2 7 0,-4-4 0,4 4 0,1 0 0,-5-4 0,11 3 0,-10 0 0,10 2 0,-3-1 0,4 5 0,0 6 0,-21 20 0,13 2 0,-22 8 0,25-11 0,-12 0 0,13-10 0,-5-3 0,9-9 0,5-8 0,-2-1 0,9-8 0,-4 0 0,5 0 0,-3-4 0,-2 3 0,-4-3 0,-2 4 0,1 0 0,0 1 0,4-1 0,-3 0 0,8 0 0,-4 0 0,1-4 0,3-2 0,-4-4 0</inkml:trace>
 </inkml:ink>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1535,11 +1531,11 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:T39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="5.75" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
@@ -1547,19 +1543,19 @@
     <col min="20" max="20" width="8" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:7" ht="31" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="76" t="s">
         <v>2</v>
       </c>
@@ -1570,7 +1566,7 @@
       <c r="F3" s="76"/>
       <c r="G3" s="76"/>
     </row>
-    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>3</v>
       </c>
@@ -1578,7 +1574,7 @@
       <c r="C4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>4</v>
       </c>
@@ -1586,7 +1582,7 @@
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>5</v>
       </c>
@@ -1594,7 +1590,7 @@
       <c r="C6" s="5"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>0</v>
       </c>
@@ -1604,7 +1600,7 @@
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1614,7 +1610,7 @@
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>2</v>
       </c>
@@ -1624,7 +1620,7 @@
       <c r="C9" s="5"/>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>3</v>
       </c>
@@ -1634,7 +1630,7 @@
       <c r="C10" s="5"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>4</v>
       </c>
@@ -1644,7 +1640,7 @@
       <c r="C11" s="5"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>5</v>
       </c>
@@ -1654,13 +1650,13 @@
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="5"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
@@ -1672,13 +1668,13 @@
       </c>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
       <c r="D15" s="10"/>
     </row>
-    <row r="16" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>14</v>
       </c>
@@ -1686,8 +1682,8 @@
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
     </row>
-    <row r="17" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="18" spans="2:20" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="17" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="18" spans="2:20" ht="16.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="E18" s="77" t="s">
@@ -1709,7 +1705,7 @@
       <c r="S18" s="78"/>
       <c r="T18" s="79"/>
     </row>
-    <row r="19" spans="2:20" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="2:20" ht="106.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="13">
@@ -1776,7 +1772,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="20" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="80" t="s">
         <v>17</v>
       </c>
@@ -1813,7 +1809,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="21" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="81"/>
       <c r="C21" s="21">
         <v>1220741</v>
@@ -1848,7 +1844,7 @@
         <v>3.8</v>
       </c>
     </row>
-    <row r="22" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="22" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B22" s="81"/>
       <c r="C22" s="21">
         <v>1221083</v>
@@ -1883,7 +1879,7 @@
         <v>4.2</v>
       </c>
     </row>
-    <row r="23" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="23" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="81"/>
       <c r="C23" s="21">
         <v>1220928</v>
@@ -1908,7 +1904,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="24" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="24" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="81"/>
       <c r="C24" s="21">
         <v>1220917</v>
@@ -1917,7 +1913,7 @@
         <v>4</v>
       </c>
       <c r="E24" s="21">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F24" s="21">
         <v>4</v>
@@ -1940,10 +1936,10 @@
       <c r="R24" s="24"/>
       <c r="S24" s="25">
         <f t="shared" si="0"/>
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="25" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+        <v>3.8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B25" s="81"/>
       <c r="C25" s="21" t="s">
         <v>18</v>
@@ -1968,7 +1964,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="26" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="26" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B26" s="81"/>
       <c r="C26" s="21" t="s">
         <v>19</v>
@@ -1993,7 +1989,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="27" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="27" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B27" s="81"/>
       <c r="C27" s="21" t="s">
         <v>20</v>
@@ -2018,7 +2014,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="28" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="28" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B28" s="81"/>
       <c r="C28" s="21" t="s">
         <v>21</v>
@@ -2043,7 +2039,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="29" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="29" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="81"/>
       <c r="C29" s="21" t="s">
         <v>22</v>
@@ -2068,7 +2064,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="30" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="30" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B30" s="81"/>
       <c r="C30" s="21" t="s">
         <v>23</v>
@@ -2093,7 +2089,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="31" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="31" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="81"/>
       <c r="C31" s="21" t="s">
         <v>24</v>
@@ -2118,7 +2114,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="32" spans="2:20" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="32" spans="2:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B32" s="81"/>
       <c r="C32" s="21" t="s">
         <v>25</v>
@@ -2143,7 +2139,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="33" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="81"/>
       <c r="C33" s="21" t="s">
         <v>26</v>
@@ -2168,7 +2164,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="34" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="82"/>
       <c r="C34" s="27" t="s">
         <v>27</v>
@@ -2193,7 +2189,7 @@
         <v>#DIV/0!</v>
       </c>
     </row>
-    <row r="35" spans="1:19" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:19" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B35" s="2"/>
       <c r="C35" s="12" t="s">
         <v>16</v>
@@ -2204,7 +2200,7 @@
       </c>
       <c r="E35" s="31">
         <f t="shared" ref="E35:R35" si="1">AVERAGE(E20:E34)</f>
-        <v>3.25</v>
+        <v>3.5</v>
       </c>
       <c r="F35" s="31">
         <f t="shared" si="1"/>
@@ -2260,10 +2256,10 @@
       </c>
       <c r="S35" s="33"/>
     </row>
-    <row r="37" spans="1:19" ht="31" x14ac:dyDescent="0.7">
+    <row r="37" spans="1:19" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A37" s="3"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39" s="34"/>
     </row>
   </sheetData>
@@ -2288,11 +2284,11 @@
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:AC18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="3" width="11" style="73"/>
     <col min="4" max="23" width="7.25" style="74" customWidth="1"/>
@@ -2304,7 +2300,7 @@
     <col min="30" max="16384" width="11" style="74"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="40" customFormat="1" ht="343.9" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:29" s="40" customFormat="1" ht="343.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35"/>
       <c r="B1" s="36"/>
       <c r="C1" s="35"/>
@@ -2385,7 +2381,7 @@
       </c>
       <c r="AC1" s="39"/>
     </row>
-    <row r="2" spans="1:29" s="40" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:29" s="40" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41" t="s">
         <v>51</v>
       </c>
@@ -2474,7 +2470,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="83" t="s">
         <v>60</v>
       </c>
@@ -2549,49 +2545,77 @@
       <c r="AB3" s="53"/>
       <c r="AC3" s="54"/>
     </row>
-    <row r="4" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="84"/>
       <c r="B4" s="84"/>
       <c r="C4" s="55">
         <v>1220917</v>
       </c>
-      <c r="D4" s="56"/>
+      <c r="D4" s="56">
+        <v>4</v>
+      </c>
       <c r="E4" s="57"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
+      <c r="F4" s="56">
+        <v>3</v>
+      </c>
+      <c r="G4" s="56">
+        <v>4</v>
+      </c>
       <c r="H4" s="57"/>
       <c r="I4" s="57"/>
       <c r="J4" s="57"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56"/>
-      <c r="Q4" s="56"/>
+      <c r="K4" s="56">
+        <v>3</v>
+      </c>
+      <c r="L4" s="56">
+        <v>4</v>
+      </c>
+      <c r="M4" s="56">
+        <v>4</v>
+      </c>
+      <c r="N4" s="56">
+        <v>4</v>
+      </c>
+      <c r="O4" s="56">
+        <v>4</v>
+      </c>
+      <c r="P4" s="56">
+        <v>4</v>
+      </c>
+      <c r="Q4" s="56">
+        <v>3</v>
+      </c>
       <c r="R4" s="57"/>
       <c r="S4" s="57"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="56"/>
+      <c r="T4" s="56">
+        <v>3</v>
+      </c>
+      <c r="U4" s="56">
+        <v>4</v>
+      </c>
+      <c r="V4" s="56">
+        <v>4</v>
+      </c>
+      <c r="W4" s="56">
+        <v>3</v>
+      </c>
       <c r="X4" s="58"/>
       <c r="Y4" s="59">
         <f>SUMPRODUCT(D2:W2,D4:W4)/5</f>
-        <v>0</v>
+        <v>0.72363636363636374</v>
       </c>
       <c r="Z4" s="60">
         <f t="shared" ref="Z4:Z8" si="0">Y4*5</f>
-        <v>0</v>
+        <v>3.6181818181818186</v>
       </c>
       <c r="AA4" s="61">
         <f t="shared" ref="AA4:AA8" si="1">MIN(ROUND(Y4*20,2),20)</f>
-        <v>0</v>
+        <v>14.47</v>
       </c>
       <c r="AB4" s="62"/>
       <c r="AC4" s="63"/>
     </row>
-    <row r="5" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="84"/>
       <c r="B5" s="84"/>
       <c r="C5" s="55">
@@ -2661,7 +2685,7 @@
       <c r="AB5" s="62"/>
       <c r="AC5" s="63"/>
     </row>
-    <row r="6" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="84"/>
       <c r="B6" s="84"/>
       <c r="C6" s="55">
@@ -2703,7 +2727,7 @@
       <c r="AB6" s="62"/>
       <c r="AC6" s="63"/>
     </row>
-    <row r="7" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="84"/>
       <c r="B7" s="84"/>
       <c r="C7" s="55">
@@ -2745,7 +2769,7 @@
       <c r="AB7" s="62"/>
       <c r="AC7" s="63"/>
     </row>
-    <row r="8" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:29" customFormat="1" ht="19.149999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="85"/>
       <c r="B8" s="85"/>
       <c r="C8" s="64"/>
@@ -2785,7 +2809,7 @@
       <c r="AB8" s="71"/>
       <c r="AC8" s="72"/>
     </row>
-    <row r="10" spans="1:29" ht="31" x14ac:dyDescent="0.7">
+    <row r="10" spans="1:29" ht="31.5" x14ac:dyDescent="0.5">
       <c r="A10" s="3" t="s">
         <v>1</v>
       </c>
@@ -2796,7 +2820,7 @@
       <c r="F10"/>
       <c r="G10"/>
     </row>
-    <row r="11" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>61</v>
       </c>
@@ -2807,7 +2831,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>62</v>
       </c>
@@ -2818,7 +2842,7 @@
       <c r="F12" s="4"/>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>0</v>
       </c>
@@ -2831,7 +2855,7 @@
       <c r="F13" s="4"/>
       <c r="G13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -2844,7 +2868,7 @@
       <c r="F14" s="4"/>
       <c r="G14" s="4"/>
     </row>
-    <row r="15" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A15" s="5">
         <v>2</v>
       </c>
@@ -2857,7 +2881,7 @@
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
     </row>
-    <row r="16" spans="1:29" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:29" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>3</v>
       </c>
@@ -2870,7 +2894,7 @@
       <c r="F16" s="4"/>
       <c r="G16" s="4"/>
     </row>
-    <row r="17" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>4</v>
       </c>
@@ -2883,7 +2907,7 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
     </row>
-    <row r="18" spans="1:7" ht="18.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>5</v>
       </c>
@@ -2913,6 +2937,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100C8B18F131359BB48BCDE011E677140C8" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7c575d82af674a11f8850f3227e50b0b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="40f68083-8b1e-401a-aff0-261d16eabb01" xmlns:ns3="6fb2d6cf-5937-415c-8e29-0a2ba0894026" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ee7e4bd6e2ea6e83e9fae13acd7478ae" ns2:_="" ns3:_="">
     <xsd:import namespace="40f68083-8b1e-401a-aff0-261d16eabb01"/>
@@ -3101,41 +3145,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="6fb2d6cf-5937-415c-8e29-0a2ba0894026" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="40f68083-8b1e-401a-aff0-261d16eabb01">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DAA54B-90F9-4C2D-87EC-856BE0A86E6D}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
-    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3158,9 +3171,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{500E29BA-14B8-49D6-A6F7-C9CFB2D16C3A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{90DAA54B-90F9-4C2D-87EC-856BE0A86E6D}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="40f68083-8b1e-401a-aff0-261d16eabb01"/>
+    <ds:schemaRef ds:uri="6fb2d6cf-5937-415c-8e29-0a2ba0894026"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>